<commit_message>
feat: Add BCI-controlled dinosaur game view and project attendance tracking files.
</commit_message>
<xml_diff>
--- a/attendance/Neurokeys - BCI Typing Project.xlsx
+++ b/attendance/Neurokeys - BCI Typing Project.xlsx
@@ -1724,7 +1724,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O3" s="22" t="inlineStr"/>
+      <c r="O3" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P3" s="22" t="inlineStr"/>
       <c r="Q3" s="22" t="inlineStr"/>
       <c r="R3" s="22" t="inlineStr"/>
@@ -1829,7 +1833,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O4" s="22" t="inlineStr"/>
+      <c r="O4" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P4" s="22" t="inlineStr"/>
       <c r="Q4" s="22" t="inlineStr"/>
       <c r="R4" s="22" t="inlineStr"/>
@@ -1934,7 +1942,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O5" s="22" t="inlineStr"/>
+      <c r="O5" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P5" s="22" t="inlineStr"/>
       <c r="Q5" s="22" t="inlineStr"/>
       <c r="R5" s="22" t="inlineStr"/>
@@ -2039,7 +2051,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O6" s="22" t="inlineStr"/>
+      <c r="O6" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P6" s="22" t="inlineStr"/>
       <c r="Q6" s="22" t="inlineStr"/>
       <c r="R6" s="22" t="inlineStr"/>
@@ -2139,12 +2155,16 @@
           <t>H</t>
         </is>
       </c>
-      <c r="N7" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="O7" s="22" t="inlineStr"/>
+      <c r="N7" s="29" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="O7" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P7" s="22" t="inlineStr"/>
       <c r="Q7" s="22" t="inlineStr"/>
       <c r="R7" s="22" t="inlineStr"/>
@@ -2249,7 +2269,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O8" s="22" t="inlineStr"/>
+      <c r="O8" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P8" s="22" t="inlineStr"/>
       <c r="Q8" s="22" t="inlineStr"/>
       <c r="R8" s="22" t="inlineStr"/>
@@ -2349,12 +2373,16 @@
           <t>H</t>
         </is>
       </c>
-      <c r="N9" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="O9" s="22" t="inlineStr"/>
+      <c r="N9" s="29" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="O9" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P9" s="22" t="inlineStr"/>
       <c r="Q9" s="22" t="inlineStr"/>
       <c r="R9" s="22" t="inlineStr"/>
@@ -2459,7 +2487,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O10" s="22" t="inlineStr"/>
+      <c r="O10" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P10" s="22" t="inlineStr"/>
       <c r="Q10" s="22" t="inlineStr"/>
       <c r="R10" s="22" t="inlineStr"/>
@@ -2564,7 +2596,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O11" s="22" t="inlineStr"/>
+      <c r="O11" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P11" s="22" t="inlineStr"/>
       <c r="Q11" s="22" t="inlineStr"/>
       <c r="R11" s="22" t="inlineStr"/>
@@ -2669,7 +2705,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O12" s="22" t="inlineStr"/>
+      <c r="O12" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P12" s="22" t="inlineStr"/>
       <c r="Q12" s="22" t="inlineStr"/>
       <c r="R12" s="22" t="inlineStr"/>
@@ -2774,7 +2814,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O13" s="22" t="inlineStr"/>
+      <c r="O13" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P13" s="22" t="inlineStr"/>
       <c r="Q13" s="22" t="inlineStr"/>
       <c r="R13" s="22" t="inlineStr"/>
@@ -2879,7 +2923,11 @@
           <t>L</t>
         </is>
       </c>
-      <c r="O14" s="22" t="inlineStr"/>
+      <c r="O14" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P14" s="22" t="inlineStr"/>
       <c r="Q14" s="22" t="inlineStr"/>
       <c r="R14" s="22" t="inlineStr"/>
@@ -2979,12 +3027,16 @@
           <t>H</t>
         </is>
       </c>
-      <c r="N15" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="O15" s="22" t="inlineStr"/>
+      <c r="N15" s="29" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="O15" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P15" s="22" t="inlineStr"/>
       <c r="Q15" s="22" t="inlineStr"/>
       <c r="R15" s="22" t="inlineStr"/>
@@ -3089,7 +3141,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O16" s="22" t="inlineStr"/>
+      <c r="O16" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P16" s="22" t="inlineStr"/>
       <c r="Q16" s="22" t="inlineStr"/>
       <c r="R16" s="22" t="inlineStr"/>
@@ -3194,7 +3250,11 @@
           <t>L</t>
         </is>
       </c>
-      <c r="O17" s="22" t="inlineStr"/>
+      <c r="O17" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P17" s="22" t="inlineStr"/>
       <c r="Q17" s="22" t="inlineStr"/>
       <c r="R17" s="22" t="inlineStr"/>
@@ -3279,9 +3339,9 @@
           <t>L</t>
         </is>
       </c>
-      <c r="K18" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
+      <c r="K18" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
         </is>
       </c>
       <c r="L18" s="24" t="inlineStr">
@@ -3299,7 +3359,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O18" s="22" t="inlineStr"/>
+      <c r="O18" s="27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="P18" s="22" t="inlineStr"/>
       <c r="Q18" s="22" t="inlineStr"/>
       <c r="R18" s="22" t="inlineStr"/>
@@ -3404,7 +3468,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="O19" s="22" t="inlineStr"/>
+      <c r="O19" s="24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="P19" s="22" t="inlineStr"/>
       <c r="Q19" s="22" t="inlineStr"/>
       <c r="R19" s="22" t="inlineStr"/>
@@ -3442,10 +3510,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:AK1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:AK1"/>
-    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="1"/>

</xml_diff>